<commit_message>
Add trabalho em grupo
</commit_message>
<xml_diff>
--- a/BaseRN.xlsx
+++ b/BaseRN.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Base RN" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Base RN'!$A$1:$AQ$165</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -647,10 +650,10 @@
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="#"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="#"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -667,6 +670,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -681,6 +692,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -690,7 +731,31 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -705,16 +770,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -729,85 +808,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -826,7 +829,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,115 +841,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -958,13 +853,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,7 +871,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,7 +967,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1006,7 +979,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1030,6 +1033,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1040,6 +1058,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1055,41 +1091,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1111,9 +1112,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1122,148 +1125,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1635,11 +1638,17 @@
   <sheetPr/>
   <dimension ref="A1:AQ165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AS4" sqref="AS2:AS4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="30" max="30" width="16.2" customWidth="1"/>
+    <col min="31" max="31" width="16" customWidth="1"/>
+    <col min="36" max="36" width="12.7" customWidth="1"/>
+    <col min="42" max="42" width="11.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
@@ -23585,6 +23594,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AQ165">
+    <extLst/>
+  </autoFilter>
   <conditionalFormatting sqref="D2">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
       <formula>$D2</formula>

</xml_diff>